<commit_message>
add lc.130, add disjoint-set of 200
</commit_message>
<xml_diff>
--- a/算法训练营题目汇总.xlsx
+++ b/算法训练营题目汇总.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-5280" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="4"/>
+    <workbookView xWindow="8780" yWindow="-21140" windowWidth="19200" windowHeight="21140" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="week5" sheetId="5" r:id="rId4"/>
     <sheet name="week6" sheetId="4" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">week5!$D$1:$D$29</definedName>
+  </definedNames>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="135">
   <si>
     <t>Array</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -385,10 +388,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>完成状态</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>第12课</t>
   </si>
   <si>
@@ -485,9 +484,6 @@
     <t>字典树和并查集</t>
   </si>
   <si>
-    <t>https://leetcode-cn.com/problems/implement-trie-prefix-tree/#/description</t>
-  </si>
-  <si>
     <t>https://leetcode-cn.com/problems/word-search-ii/</t>
   </si>
   <si>
@@ -522,6 +518,15 @@
   </si>
   <si>
     <t>https://leetcode-cn.com/problems/valid-sudoku/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/shortest-path-in-binary-matrix/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/sliding-puzzle/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/implement-trie-prefix-tree/</t>
   </si>
 </sst>
 </file>
@@ -676,7 +681,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -713,17 +718,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -755,7 +751,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1062,15 +1064,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G154"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.6640625" customWidth="1"/>
     <col min="3" max="3" width="70.1640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="4" max="5" width="10.1640625" customWidth="1"/>
+    <col min="6" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1083,70 +1086,114 @@
       <c r="C1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>88</v>
+      <c r="D1" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="E1" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="F1" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>130</v>
-      </c>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+      <c r="D2" s="15">
+        <v>43791</v>
+      </c>
+      <c r="E2" s="15">
+        <f>D2+1</f>
+        <v>43792</v>
+      </c>
+      <c r="F2" s="15">
+        <f>D2+7</f>
+        <v>43798</v>
+      </c>
+      <c r="G2" s="15">
+        <f>D2+30</f>
+        <v>43821</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="D3" s="15">
+        <v>43791</v>
+      </c>
+      <c r="E3" s="15">
+        <f t="shared" ref="E3:E5" si="0">D3+1</f>
+        <v>43792</v>
+      </c>
+      <c r="F3" s="15">
+        <f t="shared" ref="F3:F5" si="1">D3+7</f>
+        <v>43798</v>
+      </c>
+      <c r="G3" s="15">
+        <f t="shared" ref="G3:G5" si="2">D3+30</f>
+        <v>43821</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
+      <c r="D4" s="15">
+        <v>43791</v>
+      </c>
+      <c r="E4" s="15">
+        <f t="shared" si="0"/>
+        <v>43792</v>
+      </c>
+      <c r="F4" s="15">
+        <f t="shared" si="1"/>
+        <v>43798</v>
+      </c>
+      <c r="G4" s="15">
+        <f t="shared" si="2"/>
+        <v>43821</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+      <c r="D5" s="15">
+        <v>43791</v>
+      </c>
+      <c r="E5" s="15">
+        <f t="shared" si="0"/>
+        <v>43792</v>
+      </c>
+      <c r="F5" s="15">
+        <f t="shared" si="1"/>
+        <v>43798</v>
+      </c>
+      <c r="G5" s="15">
+        <f t="shared" si="2"/>
+        <v>43821</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19" t="s">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -1158,8 +1205,8 @@
       <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
@@ -1169,8 +1216,8 @@
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="5" t="s">
         <v>9</v>
       </c>
@@ -1180,8 +1227,8 @@
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1191,8 +1238,8 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="19"/>
-      <c r="B10" s="19"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="5" t="s">
         <v>12</v>
       </c>
@@ -1202,8 +1249,8 @@
       <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19" t="s">
+      <c r="A11" s="16"/>
+      <c r="B11" s="16" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -1215,8 +1262,8 @@
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
@@ -1226,8 +1273,8 @@
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1237,8 +1284,8 @@
       <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="19"/>
-      <c r="B14" s="19"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1248,8 +1295,8 @@
       <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1259,8 +1306,8 @@
       <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="5" t="s">
         <v>4</v>
       </c>
@@ -1270,8 +1317,8 @@
       <c r="G16" s="6"/>
     </row>
     <row r="17" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="5" t="s">
         <v>17</v>
       </c>
@@ -1281,10 +1328,10 @@
       <c r="G17" s="6"/>
     </row>
     <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="16" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1296,8 +1343,8 @@
       <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="7" t="s">
         <v>25</v>
       </c>
@@ -1307,8 +1354,8 @@
       <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19" t="s">
+      <c r="A20" s="16"/>
+      <c r="B20" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -1320,8 +1367,8 @@
       <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
       <c r="C21" s="7" t="s">
         <v>23</v>
       </c>
@@ -1331,8 +1378,8 @@
       <c r="G21" s="6"/>
     </row>
     <row r="22" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19" t="s">
+      <c r="A22" s="16"/>
+      <c r="B22" s="16" t="s">
         <v>2</v>
       </c>
       <c r="C22" s="7" t="s">
@@ -1344,8 +1391,8 @@
       <c r="G22" s="6"/>
     </row>
     <row r="23" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
       <c r="C23" s="7" t="s">
         <v>20</v>
       </c>
@@ -1497,11 +1544,6 @@
     <mergeCell ref="B20:B21"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
-      <formula1>"已完成,未完成"</formula1>
-    </dataValidation>
-  </dataValidations>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
@@ -1535,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:G14"/>
+    <sheetView topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1556,24 +1598,24 @@
       <c r="C1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>88</v>
+      <c r="D1" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="E1" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="F1" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>130</v>
-      </c>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="16" t="s">
         <v>52</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -1585,8 +1627,8 @@
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="7" t="s">
         <v>30</v>
       </c>
@@ -1596,8 +1638,8 @@
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="7" t="s">
         <v>30</v>
       </c>
@@ -1607,10 +1649,10 @@
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="16" t="s">
         <v>53</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1622,8 +1664,8 @@
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="7" t="s">
         <v>32</v>
       </c>
@@ -1633,8 +1675,8 @@
       <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="7" t="s">
         <v>33</v>
       </c>
@@ -1644,8 +1686,8 @@
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="7" t="s">
         <v>34</v>
       </c>
@@ -1655,8 +1697,8 @@
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="7" t="s">
         <v>35</v>
       </c>
@@ -1666,10 +1708,10 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="16" t="s">
         <v>54</v>
       </c>
       <c r="C10" s="7" t="s">
@@ -1681,8 +1723,8 @@
       <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="7" t="s">
         <v>36</v>
       </c>
@@ -1692,8 +1734,8 @@
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="7" t="s">
         <v>37</v>
       </c>
@@ -1703,8 +1745,8 @@
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="7" t="s">
         <v>38</v>
       </c>
@@ -1714,8 +1756,8 @@
       <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="19"/>
-      <c r="B14" s="19"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="7" t="s">
         <v>39</v>
       </c>
@@ -1725,8 +1767,8 @@
       <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="7" t="s">
         <v>40</v>
       </c>
@@ -1736,8 +1778,8 @@
       <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="7" t="s">
         <v>41</v>
       </c>
@@ -1747,8 +1789,8 @@
       <c r="G16" s="6"/>
     </row>
     <row r="17" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19" t="s">
+      <c r="A17" s="16"/>
+      <c r="B17" s="16" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="7" t="s">
@@ -1760,8 +1802,8 @@
       <c r="G17" s="6"/>
     </row>
     <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="19"/>
-      <c r="B18" s="19"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="7" t="s">
         <v>43</v>
       </c>
@@ -1771,8 +1813,8 @@
       <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="7" t="s">
         <v>44</v>
       </c>
@@ -1782,8 +1824,8 @@
       <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="7" t="s">
         <v>45</v>
       </c>
@@ -1793,8 +1835,8 @@
       <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
       <c r="C21" s="7" t="s">
         <v>46</v>
       </c>
@@ -1804,10 +1846,10 @@
       <c r="G21" s="6"/>
     </row>
     <row r="22" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="16" t="s">
         <v>55</v>
       </c>
       <c r="C22" s="7" t="s">
@@ -1819,8 +1861,8 @@
       <c r="G22" s="6"/>
     </row>
     <row r="23" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
       <c r="C23" s="7" t="s">
         <v>47</v>
       </c>
@@ -1830,8 +1872,8 @@
       <c r="G23" s="6"/>
     </row>
     <row r="24" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="19"/>
-      <c r="B24" s="19" t="s">
+      <c r="A24" s="16"/>
+      <c r="B24" s="16" t="s">
         <v>2</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1843,8 +1885,8 @@
       <c r="G24" s="6"/>
     </row>
     <row r="25" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="19"/>
-      <c r="B25" s="19"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
       <c r="C25" s="7" t="s">
         <v>50</v>
       </c>
@@ -1854,8 +1896,8 @@
       <c r="G25" s="6"/>
     </row>
     <row r="26" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="19"/>
-      <c r="B26" s="19"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
       <c r="C26" s="7" t="s">
         <v>51</v>
       </c>
@@ -1881,11 +1923,6 @@
     <mergeCell ref="B24:B26"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
-      <formula1>"已完成,未完成"</formula1>
-    </dataValidation>
-  </dataValidations>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
@@ -1922,8 +1959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="G14" sqref="E1:G14"/>
+    <sheetView topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1943,24 +1980,24 @@
       <c r="C1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>88</v>
+      <c r="D1" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="E1" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="F1" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>130</v>
-      </c>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="16" t="s">
         <v>83</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -1972,8 +2009,8 @@
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="7" t="s">
         <v>60</v>
       </c>
@@ -1983,8 +2020,8 @@
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="7" t="s">
         <v>61</v>
       </c>
@@ -1994,8 +2031,8 @@
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="7" t="s">
         <v>62</v>
       </c>
@@ -2005,8 +2042,8 @@
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19" t="s">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -2018,8 +2055,8 @@
       <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="7" t="s">
         <v>64</v>
       </c>
@@ -2029,8 +2066,8 @@
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="7" t="s">
         <v>65</v>
       </c>
@@ -2040,8 +2077,8 @@
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="7" t="s">
         <v>66</v>
       </c>
@@ -2051,7 +2088,7 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="16" t="s">
         <v>82</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -2066,8 +2103,8 @@
       <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19" t="s">
+      <c r="A11" s="16"/>
+      <c r="B11" s="16" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="7" t="s">
@@ -2079,8 +2116,8 @@
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="7" t="s">
         <v>69</v>
       </c>
@@ -2090,8 +2127,8 @@
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="7" t="s">
         <v>70</v>
       </c>
@@ -2101,8 +2138,8 @@
       <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="19"/>
-      <c r="B14" s="19"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="7" t="s">
         <v>71</v>
       </c>
@@ -2112,8 +2149,8 @@
       <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="7" t="s">
         <v>72</v>
       </c>
@@ -2123,8 +2160,8 @@
       <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="7" t="s">
         <v>73</v>
       </c>
@@ -2134,10 +2171,10 @@
       <c r="G16" s="6"/>
     </row>
     <row r="17" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="16" t="s">
         <v>79</v>
       </c>
       <c r="C17" s="7" t="s">
@@ -2149,8 +2186,8 @@
       <c r="G17" s="6"/>
     </row>
     <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="19"/>
-      <c r="B18" s="19"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="7" t="s">
         <v>74</v>
       </c>
@@ -2160,8 +2197,8 @@
       <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19" t="s">
+      <c r="A19" s="16"/>
+      <c r="B19" s="16" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -2173,8 +2210,8 @@
       <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="7" t="s">
         <v>77</v>
       </c>
@@ -2184,8 +2221,8 @@
       <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
       <c r="C21" s="7" t="s">
         <v>78</v>
       </c>
@@ -2210,11 +2247,6 @@
     <mergeCell ref="B6:B9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
-      <formula1>"已完成,未完成"</formula1>
-    </dataValidation>
-  </dataValidations>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
@@ -2246,8 +2278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2267,28 +2299,28 @@
       <c r="C1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
+      <c r="B2" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="C2" s="12" t="s">
         <v>90</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>91</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -2296,10 +2328,10 @@
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="23"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="14" t="s">
-        <v>92</v>
+      <c r="A3" s="20"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="12" t="s">
+        <v>91</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -2307,10 +2339,10 @@
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="23"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="14" t="s">
-        <v>93</v>
+      <c r="A4" s="20"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="12" t="s">
+        <v>92</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -2318,10 +2350,10 @@
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="23"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="14" t="s">
-        <v>107</v>
+      <c r="A5" s="20"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="12" t="s">
+        <v>106</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -2329,10 +2361,10 @@
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="23"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="14" t="s">
-        <v>108</v>
+      <c r="A6" s="20"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="12" t="s">
+        <v>107</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -2340,10 +2372,10 @@
       <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="23"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="14" t="s">
-        <v>109</v>
+      <c r="A7" s="20"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="12" t="s">
+        <v>108</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="6"/>
@@ -2351,10 +2383,10 @@
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="23"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="14" t="s">
-        <v>110</v>
+      <c r="A8" s="20"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="12" t="s">
+        <v>109</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="6"/>
@@ -2362,10 +2394,10 @@
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="23"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="14" t="s">
-        <v>111</v>
+      <c r="A9" s="20"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="12" t="s">
+        <v>110</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="6"/>
@@ -2373,10 +2405,10 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="23"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="14" t="s">
-        <v>112</v>
+      <c r="A10" s="20"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="12" t="s">
+        <v>111</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -2384,10 +2416,10 @@
       <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="23"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="14" t="s">
-        <v>113</v>
+      <c r="A11" s="20"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="12" t="s">
+        <v>112</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -2395,10 +2427,10 @@
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="23"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="14" t="s">
-        <v>114</v>
+      <c r="A12" s="20"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="12" t="s">
+        <v>113</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -2406,10 +2438,10 @@
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="23"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="14" t="s">
-        <v>115</v>
+      <c r="A13" s="20"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="12" t="s">
+        <v>114</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -2417,10 +2449,10 @@
       <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="23"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="14" t="s">
-        <v>116</v>
+      <c r="A14" s="20"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="12" t="s">
+        <v>115</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -2428,10 +2460,10 @@
       <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="23"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="14" t="s">
-        <v>117</v>
+      <c r="A15" s="20"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="12" t="s">
+        <v>116</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -2439,10 +2471,10 @@
       <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="23"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="14" t="s">
-        <v>118</v>
+      <c r="A16" s="20"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="12" t="s">
+        <v>117</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -2450,12 +2482,12 @@
       <c r="G16" s="6"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="23"/>
-      <c r="B17" s="19" t="s">
+      <c r="A17" s="20"/>
+      <c r="B17" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="14" t="s">
-        <v>94</v>
+      <c r="C17" s="12" t="s">
+        <v>93</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -2463,10 +2495,10 @@
       <c r="G17" s="6"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="23"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="14" t="s">
-        <v>95</v>
+      <c r="A18" s="20"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="12" t="s">
+        <v>94</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -2474,10 +2506,10 @@
       <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="23"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="14" t="s">
-        <v>96</v>
+      <c r="A19" s="20"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="12" t="s">
+        <v>95</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -2485,10 +2517,10 @@
       <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="23"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="14" t="s">
-        <v>97</v>
+      <c r="A20" s="20"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="12" t="s">
+        <v>96</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="6"/>
@@ -2496,10 +2528,10 @@
       <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="23"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="14" t="s">
-        <v>98</v>
+      <c r="A21" s="20"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="6"/>
@@ -2507,10 +2539,10 @@
       <c r="G21" s="6"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="23"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="14" t="s">
-        <v>99</v>
+      <c r="A22" s="20"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="12" t="s">
+        <v>98</v>
       </c>
       <c r="D22" s="10"/>
       <c r="E22" s="6"/>
@@ -2518,10 +2550,10 @@
       <c r="G22" s="6"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="23"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="14" t="s">
-        <v>100</v>
+      <c r="A23" s="20"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="12" t="s">
+        <v>99</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="6"/>
@@ -2529,10 +2561,10 @@
       <c r="G23" s="6"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="23"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="14" t="s">
-        <v>101</v>
+      <c r="A24" s="20"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="12" t="s">
+        <v>100</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="6"/>
@@ -2540,10 +2572,10 @@
       <c r="G24" s="6"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="23"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="14" t="s">
-        <v>102</v>
+      <c r="A25" s="20"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="12" t="s">
+        <v>101</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="6"/>
@@ -2551,10 +2583,10 @@
       <c r="G25" s="6"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="23"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="14" t="s">
-        <v>103</v>
+      <c r="A26" s="20"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="12" t="s">
+        <v>102</v>
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="6"/>
@@ -2562,10 +2594,10 @@
       <c r="G26" s="6"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="23"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="14" t="s">
-        <v>104</v>
+      <c r="A27" s="20"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="12" t="s">
+        <v>103</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="6"/>
@@ -2573,10 +2605,10 @@
       <c r="G27" s="6"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="23"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="14" t="s">
-        <v>105</v>
+      <c r="A28" s="20"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="12" t="s">
+        <v>104</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="6"/>
@@ -2584,10 +2616,10 @@
       <c r="G28" s="6"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="24"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="14" t="s">
-        <v>106</v>
+      <c r="A29" s="21"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="D29" s="10"/>
       <c r="E29" s="6"/>
@@ -2601,11 +2633,6 @@
     <mergeCell ref="A2:A29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D9 D20:D29">
-      <formula1>"已完成,未完成"</formula1>
-    </dataValidation>
-  </dataValidations>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
@@ -2637,6 +2664,7 @@
     <hyperlink ref="C16" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2644,15 +2672,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21:F22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
     <col min="3" max="3" width="86.5" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -2666,29 +2695,29 @@
         <v>26</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E1" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="F1" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>130</v>
-      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="D2" s="18">
+      <c r="C2" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="15">
         <v>43789</v>
       </c>
       <c r="E2" s="6"/>
@@ -2696,12 +2725,12 @@
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="D3" s="18">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" s="15">
         <v>43789</v>
       </c>
       <c r="E3" s="6"/>
@@ -2709,62 +2738,70 @@
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="D4" s="18">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" s="15">
         <v>43789</v>
       </c>
-      <c r="E4" s="6"/>
+      <c r="E4" s="15">
+        <v>43791</v>
+      </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="D5" s="18">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="15">
         <v>43789</v>
       </c>
-      <c r="E5" s="6"/>
+      <c r="E5" s="15">
+        <v>43791</v>
+      </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="D6" s="6"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="15">
+        <v>43791</v>
+      </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="D7" s="6"/>
+      <c r="A7" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" s="15">
+        <v>43791</v>
+      </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="19"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="26" t="s">
-        <v>132</v>
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="12" t="s">
+        <v>130</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -2772,114 +2809,122 @@
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="19"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="7"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="12" t="s">
+        <v>132</v>
+      </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="19"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="7"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="12" t="s">
+        <v>133</v>
+      </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="22"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="17"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="14"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="17"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="14"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="16"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="17"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="14"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="16"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="17"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="14"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="16"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="17"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="14"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="16"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="17"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="14"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="16"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="17"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="14"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="25"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="17"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="14"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="25"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="17"/>
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="14"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="25"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="17"/>
+      <c r="A24" s="22"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="14"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="25"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="17"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="14"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="25"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="17"/>
+      <c r="A26" s="22"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2888,19 +2933,21 @@
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B7:B9"/>
     <mergeCell ref="B17:B21"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="A7:A10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" location="/description"/>
+    <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3"/>
     <hyperlink ref="C5" r:id="rId4"/>
     <hyperlink ref="C6" r:id="rId5"/>
     <hyperlink ref="C7" r:id="rId6"/>
     <hyperlink ref="C8" r:id="rId7"/>
+    <hyperlink ref="C9" r:id="rId8"/>
+    <hyperlink ref="C10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update excel of week 7
</commit_message>
<xml_diff>
--- a/算法训练营题目汇总.xlsx
+++ b/算法训练营题目汇总.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8780" yWindow="-21140" windowWidth="19200" windowHeight="21140" activeTab="4"/>
+    <workbookView xWindow="13920" yWindow="-21140" windowWidth="19200" windowHeight="21140"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -17,11 +17,12 @@
     <sheet name="week3" sheetId="3" r:id="rId3"/>
     <sheet name="week5" sheetId="5" r:id="rId4"/>
     <sheet name="week6" sheetId="4" r:id="rId5"/>
+    <sheet name="week7" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">week5!$D$1:$D$29</definedName>
   </definedNames>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="150">
   <si>
     <t>Array</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -527,6 +528,51 @@
   </si>
   <si>
     <t>https://leetcode-cn.com/problems/implement-trie-prefix-tree/</t>
+  </si>
+  <si>
+    <t>位运算</t>
+  </si>
+  <si>
+    <t>布隆过滤器和LRU缓存</t>
+  </si>
+  <si>
+    <t>排序算法</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/number-of-1-bits/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/power-of-two/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/reverse-bits/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/n-queens/description/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/n-queens-ii/description/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/counting-bits/description/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/lru-cache/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/relative-sort-array/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/valid-anagram/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/design-a-leaderboard/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/merge-intervals/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/reverse-pairs/</t>
   </si>
 </sst>
 </file>
@@ -730,6 +776,15 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -750,15 +805,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1064,8 +1110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G154"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1100,10 +1146,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -1126,74 +1172,41 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="15">
-        <v>43791</v>
-      </c>
-      <c r="E3" s="15">
-        <f t="shared" ref="E3:E5" si="0">D3+1</f>
-        <v>43792</v>
-      </c>
-      <c r="F3" s="15">
-        <f t="shared" ref="F3:F5" si="1">D3+7</f>
-        <v>43798</v>
-      </c>
-      <c r="G3" s="15">
-        <f t="shared" ref="G3:G5" si="2">D3+30</f>
-        <v>43821</v>
-      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
     </row>
     <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="15">
-        <v>43791</v>
-      </c>
-      <c r="E4" s="15">
-        <f t="shared" si="0"/>
-        <v>43792</v>
-      </c>
-      <c r="F4" s="15">
-        <f t="shared" si="1"/>
-        <v>43798</v>
-      </c>
-      <c r="G4" s="15">
-        <f t="shared" si="2"/>
-        <v>43821</v>
-      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
     </row>
     <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="15">
-        <v>43791</v>
-      </c>
-      <c r="E5" s="15">
-        <f t="shared" si="0"/>
-        <v>43792</v>
-      </c>
-      <c r="F5" s="15">
-        <f t="shared" si="1"/>
-        <v>43798</v>
-      </c>
-      <c r="G5" s="15">
-        <f t="shared" si="2"/>
-        <v>43821</v>
-      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
     </row>
     <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16" t="s">
+      <c r="A6" s="19"/>
+      <c r="B6" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -1205,8 +1218,8 @@
       <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
@@ -1216,8 +1229,8 @@
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="5" t="s">
         <v>9</v>
       </c>
@@ -1227,8 +1240,8 @@
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1238,8 +1251,8 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="19"/>
       <c r="C10" s="5" t="s">
         <v>12</v>
       </c>
@@ -1249,8 +1262,8 @@
       <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16" t="s">
+      <c r="A11" s="19"/>
+      <c r="B11" s="19" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -1262,8 +1275,8 @@
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
       <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
@@ -1273,8 +1286,8 @@
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1284,8 +1297,8 @@
       <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1295,8 +1308,8 @@
       <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
       <c r="C15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1306,8 +1319,8 @@
       <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
       <c r="C16" s="5" t="s">
         <v>4</v>
       </c>
@@ -1317,8 +1330,8 @@
       <c r="G16" s="6"/>
     </row>
     <row r="17" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
       <c r="C17" s="5" t="s">
         <v>17</v>
       </c>
@@ -1328,10 +1341,10 @@
       <c r="G17" s="6"/>
     </row>
     <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="19" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1343,8 +1356,8 @@
       <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
       <c r="C19" s="7" t="s">
         <v>25</v>
       </c>
@@ -1354,8 +1367,8 @@
       <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="16"/>
-      <c r="B20" s="16" t="s">
+      <c r="A20" s="19"/>
+      <c r="B20" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -1367,8 +1380,8 @@
       <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="16"/>
-      <c r="B21" s="16"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
       <c r="C21" s="7" t="s">
         <v>23</v>
       </c>
@@ -1378,8 +1391,8 @@
       <c r="G21" s="6"/>
     </row>
     <row r="22" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="16"/>
-      <c r="B22" s="16" t="s">
+      <c r="A22" s="19"/>
+      <c r="B22" s="19" t="s">
         <v>2</v>
       </c>
       <c r="C22" s="7" t="s">
@@ -1391,8 +1404,8 @@
       <c r="G22" s="6"/>
     </row>
     <row r="23" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
       <c r="C23" s="7" t="s">
         <v>20</v>
       </c>
@@ -1612,10 +1625,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="19" t="s">
         <v>52</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -1627,8 +1640,8 @@
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="7" t="s">
         <v>30</v>
       </c>
@@ -1638,8 +1651,8 @@
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="7" t="s">
         <v>30</v>
       </c>
@@ -1649,10 +1662,10 @@
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="19" t="s">
         <v>53</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1664,8 +1677,8 @@
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
       <c r="C6" s="7" t="s">
         <v>32</v>
       </c>
@@ -1675,8 +1688,8 @@
       <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="7" t="s">
         <v>33</v>
       </c>
@@ -1686,8 +1699,8 @@
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="7" t="s">
         <v>34</v>
       </c>
@@ -1697,8 +1710,8 @@
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="7" t="s">
         <v>35</v>
       </c>
@@ -1708,10 +1721,10 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="19" t="s">
         <v>54</v>
       </c>
       <c r="C10" s="7" t="s">
@@ -1723,8 +1736,8 @@
       <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
       <c r="C11" s="7" t="s">
         <v>36</v>
       </c>
@@ -1734,8 +1747,8 @@
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
       <c r="C12" s="7" t="s">
         <v>37</v>
       </c>
@@ -1745,8 +1758,8 @@
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="7" t="s">
         <v>38</v>
       </c>
@@ -1756,8 +1769,8 @@
       <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="7" t="s">
         <v>39</v>
       </c>
@@ -1767,8 +1780,8 @@
       <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
       <c r="C15" s="7" t="s">
         <v>40</v>
       </c>
@@ -1778,8 +1791,8 @@
       <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
       <c r="C16" s="7" t="s">
         <v>41</v>
       </c>
@@ -1789,8 +1802,8 @@
       <c r="G16" s="6"/>
     </row>
     <row r="17" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16" t="s">
+      <c r="A17" s="19"/>
+      <c r="B17" s="19" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="7" t="s">
@@ -1802,8 +1815,8 @@
       <c r="G17" s="6"/>
     </row>
     <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
       <c r="C18" s="7" t="s">
         <v>43</v>
       </c>
@@ -1813,8 +1826,8 @@
       <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
       <c r="C19" s="7" t="s">
         <v>44</v>
       </c>
@@ -1824,8 +1837,8 @@
       <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="16"/>
-      <c r="B20" s="16"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
       <c r="C20" s="7" t="s">
         <v>45</v>
       </c>
@@ -1835,8 +1848,8 @@
       <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="16"/>
-      <c r="B21" s="16"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
       <c r="C21" s="7" t="s">
         <v>46</v>
       </c>
@@ -1846,10 +1859,10 @@
       <c r="G21" s="6"/>
     </row>
     <row r="22" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="19" t="s">
         <v>55</v>
       </c>
       <c r="C22" s="7" t="s">
@@ -1861,8 +1874,8 @@
       <c r="G22" s="6"/>
     </row>
     <row r="23" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
       <c r="C23" s="7" t="s">
         <v>47</v>
       </c>
@@ -1872,8 +1885,8 @@
       <c r="G23" s="6"/>
     </row>
     <row r="24" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="16"/>
-      <c r="B24" s="16" t="s">
+      <c r="A24" s="19"/>
+      <c r="B24" s="19" t="s">
         <v>2</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1885,8 +1898,8 @@
       <c r="G24" s="6"/>
     </row>
     <row r="25" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="16"/>
-      <c r="B25" s="16"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
       <c r="C25" s="7" t="s">
         <v>50</v>
       </c>
@@ -1896,8 +1909,8 @@
       <c r="G25" s="6"/>
     </row>
     <row r="26" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="16"/>
-      <c r="B26" s="16"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
       <c r="C26" s="7" t="s">
         <v>51</v>
       </c>
@@ -1994,10 +2007,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="19" t="s">
         <v>83</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -2009,8 +2022,8 @@
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="7" t="s">
         <v>60</v>
       </c>
@@ -2020,8 +2033,8 @@
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="7" t="s">
         <v>61</v>
       </c>
@@ -2031,8 +2044,8 @@
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="7" t="s">
         <v>62</v>
       </c>
@@ -2042,8 +2055,8 @@
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16" t="s">
+      <c r="A6" s="19"/>
+      <c r="B6" s="19" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -2055,8 +2068,8 @@
       <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="7" t="s">
         <v>64</v>
       </c>
@@ -2066,8 +2079,8 @@
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="7" t="s">
         <v>65</v>
       </c>
@@ -2077,8 +2090,8 @@
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="7" t="s">
         <v>66</v>
       </c>
@@ -2088,7 +2101,7 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="19" t="s">
         <v>82</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -2103,8 +2116,8 @@
       <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16" t="s">
+      <c r="A11" s="19"/>
+      <c r="B11" s="19" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="7" t="s">
@@ -2116,8 +2129,8 @@
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
       <c r="C12" s="7" t="s">
         <v>69</v>
       </c>
@@ -2127,8 +2140,8 @@
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="7" t="s">
         <v>70</v>
       </c>
@@ -2138,8 +2151,8 @@
       <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="7" t="s">
         <v>71</v>
       </c>
@@ -2149,8 +2162,8 @@
       <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
       <c r="C15" s="7" t="s">
         <v>72</v>
       </c>
@@ -2160,8 +2173,8 @@
       <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
       <c r="C16" s="7" t="s">
         <v>73</v>
       </c>
@@ -2171,10 +2184,10 @@
       <c r="G16" s="6"/>
     </row>
     <row r="17" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="19" t="s">
         <v>79</v>
       </c>
       <c r="C17" s="7" t="s">
@@ -2186,8 +2199,8 @@
       <c r="G17" s="6"/>
     </row>
     <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
       <c r="C18" s="7" t="s">
         <v>74</v>
       </c>
@@ -2197,8 +2210,8 @@
       <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16" t="s">
+      <c r="A19" s="19"/>
+      <c r="B19" s="19" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -2210,8 +2223,8 @@
       <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="16"/>
-      <c r="B20" s="16"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
       <c r="C20" s="7" t="s">
         <v>77</v>
       </c>
@@ -2221,8 +2234,8 @@
       <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="16"/>
-      <c r="B21" s="16"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
       <c r="C21" s="7" t="s">
         <v>78</v>
       </c>
@@ -2313,10 +2326,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="20" t="s">
         <v>89</v>
       </c>
       <c r="C2" s="12" t="s">
@@ -2328,8 +2341,8 @@
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="20"/>
-      <c r="B3" s="18"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="21"/>
       <c r="C3" s="12" t="s">
         <v>91</v>
       </c>
@@ -2339,8 +2352,8 @@
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="20"/>
-      <c r="B4" s="18"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="12" t="s">
         <v>92</v>
       </c>
@@ -2350,8 +2363,8 @@
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="20"/>
-      <c r="B5" s="18"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="12" t="s">
         <v>106</v>
       </c>
@@ -2361,8 +2374,8 @@
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="20"/>
-      <c r="B6" s="18"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="21"/>
       <c r="C6" s="12" t="s">
         <v>107</v>
       </c>
@@ -2372,8 +2385,8 @@
       <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="20"/>
-      <c r="B7" s="18"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="12" t="s">
         <v>108</v>
       </c>
@@ -2383,8 +2396,8 @@
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="20"/>
-      <c r="B8" s="18"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="12" t="s">
         <v>109</v>
       </c>
@@ -2394,8 +2407,8 @@
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="20"/>
-      <c r="B9" s="18"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="12" t="s">
         <v>110</v>
       </c>
@@ -2405,8 +2418,8 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="20"/>
-      <c r="B10" s="18"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="21"/>
       <c r="C10" s="12" t="s">
         <v>111</v>
       </c>
@@ -2416,8 +2429,8 @@
       <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="20"/>
-      <c r="B11" s="18"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="21"/>
       <c r="C11" s="12" t="s">
         <v>112</v>
       </c>
@@ -2427,8 +2440,8 @@
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="20"/>
-      <c r="B12" s="18"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="21"/>
       <c r="C12" s="12" t="s">
         <v>113</v>
       </c>
@@ -2438,8 +2451,8 @@
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="20"/>
-      <c r="B13" s="18"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="21"/>
       <c r="C13" s="12" t="s">
         <v>114</v>
       </c>
@@ -2449,8 +2462,8 @@
       <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="20"/>
-      <c r="B14" s="18"/>
+      <c r="A14" s="23"/>
+      <c r="B14" s="21"/>
       <c r="C14" s="12" t="s">
         <v>115</v>
       </c>
@@ -2460,8 +2473,8 @@
       <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="20"/>
-      <c r="B15" s="18"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="21"/>
       <c r="C15" s="12" t="s">
         <v>116</v>
       </c>
@@ -2471,8 +2484,8 @@
       <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="20"/>
-      <c r="B16" s="18"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="21"/>
       <c r="C16" s="12" t="s">
         <v>117</v>
       </c>
@@ -2482,8 +2495,8 @@
       <c r="G16" s="6"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="20"/>
-      <c r="B17" s="16" t="s">
+      <c r="A17" s="23"/>
+      <c r="B17" s="19" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="12" t="s">
@@ -2495,8 +2508,8 @@
       <c r="G17" s="6"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="20"/>
-      <c r="B18" s="16"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="19"/>
       <c r="C18" s="12" t="s">
         <v>94</v>
       </c>
@@ -2506,8 +2519,8 @@
       <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="20"/>
-      <c r="B19" s="16"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="19"/>
       <c r="C19" s="12" t="s">
         <v>95</v>
       </c>
@@ -2517,8 +2530,8 @@
       <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="20"/>
-      <c r="B20" s="16"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="19"/>
       <c r="C20" s="12" t="s">
         <v>96</v>
       </c>
@@ -2528,8 +2541,8 @@
       <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="20"/>
-      <c r="B21" s="16"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="19"/>
       <c r="C21" s="12" t="s">
         <v>97</v>
       </c>
@@ -2539,8 +2552,8 @@
       <c r="G21" s="6"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="20"/>
-      <c r="B22" s="16"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="19"/>
       <c r="C22" s="12" t="s">
         <v>98</v>
       </c>
@@ -2550,8 +2563,8 @@
       <c r="G22" s="6"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
-      <c r="B23" s="16"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="19"/>
       <c r="C23" s="12" t="s">
         <v>99</v>
       </c>
@@ -2561,8 +2574,8 @@
       <c r="G23" s="6"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="20"/>
-      <c r="B24" s="16"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="19"/>
       <c r="C24" s="12" t="s">
         <v>100</v>
       </c>
@@ -2572,8 +2585,8 @@
       <c r="G24" s="6"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="20"/>
-      <c r="B25" s="16"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="19"/>
       <c r="C25" s="12" t="s">
         <v>101</v>
       </c>
@@ -2583,8 +2596,8 @@
       <c r="G25" s="6"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="20"/>
-      <c r="B26" s="16"/>
+      <c r="A26" s="23"/>
+      <c r="B26" s="19"/>
       <c r="C26" s="12" t="s">
         <v>102</v>
       </c>
@@ -2594,8 +2607,8 @@
       <c r="G26" s="6"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="20"/>
-      <c r="B27" s="16"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="19"/>
       <c r="C27" s="12" t="s">
         <v>103</v>
       </c>
@@ -2605,8 +2618,8 @@
       <c r="G27" s="6"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="20"/>
-      <c r="B28" s="16"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="12" t="s">
         <v>104</v>
       </c>
@@ -2616,8 +2629,8 @@
       <c r="G28" s="6"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="21"/>
-      <c r="B29" s="16"/>
+      <c r="A29" s="24"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="12" t="s">
         <v>105</v>
       </c>
@@ -2672,8 +2685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2708,10 +2721,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="19" t="s">
         <v>119</v>
       </c>
       <c r="C2" s="12" t="s">
@@ -2725,8 +2738,8 @@
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="12" t="s">
         <v>120</v>
       </c>
@@ -2738,8 +2751,8 @@
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="12" t="s">
         <v>121</v>
       </c>
@@ -2753,8 +2766,8 @@
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="12" t="s">
         <v>122</v>
       </c>
@@ -2768,8 +2781,8 @@
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
       <c r="C6" s="12" t="s">
         <v>123</v>
       </c>
@@ -2781,10 +2794,10 @@
       <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="19" t="s">
         <v>125</v>
       </c>
       <c r="C7" s="12" t="s">
@@ -2798,8 +2811,8 @@
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="12" t="s">
         <v>130</v>
       </c>
@@ -2809,8 +2822,8 @@
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="12" t="s">
         <v>132</v>
       </c>
@@ -2820,8 +2833,8 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="19"/>
       <c r="C10" s="12" t="s">
         <v>133</v>
       </c>
@@ -2831,40 +2844,40 @@
       <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="23"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="14"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="14"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
       <c r="B14" s="13"/>
       <c r="C14" s="14"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
@@ -2878,52 +2891,52 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
-      <c r="B17" s="22"/>
+      <c r="B17" s="25"/>
       <c r="C17" s="14"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="13"/>
-      <c r="B18" s="22"/>
+      <c r="B18" s="25"/>
       <c r="C18" s="14"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="13"/>
-      <c r="B19" s="22"/>
+      <c r="B19" s="25"/>
       <c r="C19" s="14"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="13"/>
-      <c r="B20" s="22"/>
+      <c r="B20" s="25"/>
       <c r="C20" s="14"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="13"/>
-      <c r="B21" s="22"/>
+      <c r="B21" s="25"/>
       <c r="C21" s="14"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="25"/>
       <c r="C22" s="14"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="25"/>
       <c r="C23" s="14"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="25"/>
       <c r="C24" s="14"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="25"/>
       <c r="C25" s="14"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="22"/>
-      <c r="B26" s="22"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="25"/>
       <c r="C26" s="14"/>
     </row>
   </sheetData>
@@ -2951,4 +2964,189 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="86.5" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="19"/>
+      <c r="B3" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="19"/>
+      <c r="B4" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="19"/>
+      <c r="B5" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="19"/>
+      <c r="B6" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="19"/>
+      <c r="B7" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="19"/>
+      <c r="B10" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="19"/>
+      <c r="B11" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="19"/>
+      <c r="B12" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="19"/>
+      <c r="B13" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A9:A13"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B9" r:id="rId8"/>
+    <hyperlink ref="B10" r:id="rId9"/>
+    <hyperlink ref="B11" r:id="rId10"/>
+    <hyperlink ref="B12" r:id="rId11"/>
+    <hyperlink ref="B13" r:id="rId12"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>